<commit_message>
Set up Streamlit version
Created separate command line and Streamlit versions.
</commit_message>
<xml_diff>
--- a/file_input/output.xlsx
+++ b/file_input/output.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Test1.txt_1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Test2.txt_2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Test3.txt_3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="test1.txt_1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="test2.txt_2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="other_file_name.txt_3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,7 +426,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>today</t>
+          <t>this</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -436,22 +436,24 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>the</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>from</t>
+          <t>first</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>test1</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
           <t>file</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>test1.txt</t>
         </is>
       </c>
     </row>
@@ -466,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,32 +479,65 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>from</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>test2</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+          <t>second</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
         <is>
           <t>file</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>today</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>test2.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>this</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>is</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>2sday</t>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>the</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>second</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>file</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>the</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>second</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>one</t>
         </is>
       </c>
     </row>
@@ -517,7 +552,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,37 +563,91 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>from</t>
+          <t>the</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>test3</t>
+          <t>file</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>can</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>have</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>other</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>file</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>today</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>is</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>day</t>
-        </is>
-      </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>names</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>it</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>has</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>to</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>end</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>.txt</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>(that</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>can</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>also</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>change)</t>
         </is>
       </c>
     </row>

</xml_diff>